<commit_message>
Izmene u modelu baze
</commit_message>
<xml_diff>
--- a/ModelovanjeBaze/PIZZA- relacioni.xlsx
+++ b/ModelovanjeBaze/PIZZA- relacioni.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>PIZZA:</t>
   </si>
@@ -30,18 +30,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Datum_isporuke</t>
-  </si>
-  <si>
-    <t>Vreme_isporuke</t>
-  </si>
-  <si>
-    <t>Datum_kreiranja</t>
-  </si>
-  <si>
-    <t>Vreme_kreiranja</t>
-  </si>
-  <si>
     <t>STRANI JEZIK:</t>
   </si>
   <si>
@@ -223,6 +211,12 @@
   </si>
   <si>
     <t>Id_surogat_kategorija</t>
+  </si>
+  <si>
+    <t>Datum_Vreme_isporuke</t>
+  </si>
+  <si>
+    <t>Datum_Vreme_kreiranja</t>
   </si>
 </sst>
 </file>
@@ -288,7 +282,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -324,19 +318,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -361,9 +342,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,6 +374,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,40 +681,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -743,329 +724,325 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>9</v>
+      <c r="A4" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="7" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-    </row>
-    <row r="7" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
     </row>
     <row r="10" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>43</v>
+      <c r="A10" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>10</v>
+      <c r="A13" s="15" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="H14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="K14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="D17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" s="3" t="s">
+      <c r="F17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="N14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O14" s="3" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q14" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="B20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="D20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>30</v>
+      <c r="A22" s="15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>33</v>
+      <c r="A31" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>34</v>
+        <v>59</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>36</v>
+        <v>58</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
-        <v>37</v>
+      <c r="A37" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>